<commit_message>
v0.06c - SPI changes made to tc72 and accelerometer, refer changelog
</commit_message>
<xml_diff>
--- a/Source Code/MemoryMap.xlsx
+++ b/Source Code/MemoryMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="202">
   <si>
     <t>SS</t>
   </si>
@@ -615,13 +615,28 @@
   </si>
   <si>
     <t>LOP_YELLOW</t>
+  </si>
+  <si>
+    <t>Possible SS3</t>
+  </si>
+  <si>
+    <t>Possible SS4</t>
+  </si>
+  <si>
+    <t>Possible SS5</t>
+  </si>
+  <si>
+    <t>SS2</t>
+  </si>
+  <si>
+    <t>SS1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,6 +661,12 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -852,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -867,7 +888,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -876,6 +896,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1159,7 +1182,7 @@
   <dimension ref="A2:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,15 +1196,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1230,7 +1253,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1243,7 +1266,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1256,7 +1279,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1269,7 +1292,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1282,7 +1305,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1295,20 +1318,20 @@
       <c r="D10" s="2"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1331,7 +1354,9 @@
       <c r="F12" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
@@ -1350,7 +1375,7 @@
       <c r="F13" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -1369,7 +1394,7 @@
       <c r="F14" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
@@ -1388,7 +1413,7 @@
       <c r="F15" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
@@ -1407,7 +1432,9 @@
       <c r="F16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="20" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
@@ -1426,7 +1453,9 @@
       <c r="F17" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="22" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -1445,26 +1474,30 @@
       <c r="F18" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="18" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="G19" s="18"/>
+      <c r="G19" s="18" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -1490,7 +1523,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1503,7 +1536,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1516,7 +1549,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1529,7 +1562,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1542,7 +1575,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1555,20 +1588,20 @@
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="19" t="s">
+      <c r="G26" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1596,7 +1629,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="19" t="s">
+      <c r="G29" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1617,7 +1650,7 @@
       <c r="F30" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G30" s="19" t="s">
+      <c r="G30" s="18" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1638,7 +1671,7 @@
       <c r="F31" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="18" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1651,7 +1684,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1664,7 +1697,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1677,20 +1710,20 @@
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="19" t="s">
+      <c r="G34" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16" t="s">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18" t="s">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1732,7 +1765,7 @@
       <c r="F37" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
@@ -1743,7 +1776,7 @@
       <c r="D38" s="1"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1756,7 +1789,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1769,7 +1802,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="19" t="s">
+      <c r="G40" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1782,7 +1815,7 @@
       <c r="D41" s="1"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1795,20 +1828,20 @@
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="19" t="s">
+      <c r="G42" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="18" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1836,7 +1869,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="19" t="s">
+      <c r="G45" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1849,7 +1882,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="19" t="s">
+      <c r="G46" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1862,7 +1895,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1875,7 +1908,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="19" t="s">
+      <c r="G48" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1888,7 +1921,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="19" t="s">
+      <c r="G49" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1901,20 +1934,20 @@
       <c r="D50" s="1"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="19" t="s">
+      <c r="G50" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="16" t="s">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18" t="s">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1942,7 +1975,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="19" t="s">
+      <c r="G53" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1955,7 +1988,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="19" t="s">
+      <c r="G54" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1968,7 +2001,7 @@
       <c r="D55" s="1"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="19" t="s">
+      <c r="G55" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1981,7 +2014,7 @@
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="19" t="s">
+      <c r="G56" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1994,7 +2027,7 @@
       <c r="D57" s="1"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="19" t="s">
+      <c r="G57" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2007,20 +2040,20 @@
       <c r="D58" s="2"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
-      <c r="G58" s="19" t="s">
+      <c r="G58" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="15"/>
+      <c r="A59" s="14"/>
       <c r="B59" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="18" t="s">
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2048,7 +2081,7 @@
       <c r="D61" s="1"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2061,7 +2094,7 @@
       <c r="D62" s="1"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2074,7 +2107,7 @@
       <c r="D63" s="1"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="19" t="s">
+      <c r="G63" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2087,7 +2120,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="19" t="s">
+      <c r="G64" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2100,7 +2133,7 @@
       <c r="D65" s="1"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2113,20 +2146,20 @@
       <c r="D66" s="1"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="G66" s="19" t="s">
+      <c r="G66" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="15"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="18" t="s">
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2154,7 +2187,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
-      <c r="G69" s="19" t="s">
+      <c r="G69" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2167,7 +2200,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="19" t="s">
+      <c r="G70" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2180,7 +2213,7 @@
       <c r="D71" s="1"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
-      <c r="G71" s="19" t="s">
+      <c r="G71" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2193,7 +2226,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
-      <c r="G72" s="19" t="s">
+      <c r="G72" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2206,7 +2239,7 @@
       <c r="D73" s="1"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
-      <c r="G73" s="19" t="s">
+      <c r="G73" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2219,20 +2252,20 @@
       <c r="D74" s="1"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="19" t="s">
+      <c r="G74" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="15"/>
+      <c r="A75" s="14"/>
       <c r="B75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C75" s="16"/>
-      <c r="D75" s="16"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="18" t="s">
+      <c r="C75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2276,7 +2309,7 @@
       <c r="F77" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G77" s="19" t="s">
+      <c r="G77" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2297,7 +2330,7 @@
       <c r="F78" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G78" s="19" t="s">
+      <c r="G78" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2318,7 +2351,7 @@
       <c r="F79" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G79" s="19" t="s">
+      <c r="G79" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2339,7 +2372,7 @@
       <c r="F80" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G80" s="19" t="s">
+      <c r="G80" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2360,7 +2393,7 @@
       <c r="F81" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="G81" s="19" t="s">
+      <c r="G81" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2373,20 +2406,20 @@
       <c r="D82" s="2"/>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
-      <c r="G82" s="19" t="s">
+      <c r="G82" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="15"/>
+      <c r="A83" s="14"/>
       <c r="B83" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="18" t="s">
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2428,7 +2461,7 @@
       <c r="F85" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G85" s="19"/>
+      <c r="G85" s="18"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
@@ -2447,7 +2480,7 @@
       <c r="F86" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G86" s="19"/>
+      <c r="G86" s="18"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
@@ -2466,7 +2499,7 @@
       <c r="F87" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G87" s="19"/>
+      <c r="G87" s="18"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
@@ -2526,15 +2559,15 @@
       <c r="G90" s="12"/>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="15"/>
-      <c r="B91" s="16" t="s">
+      <c r="A91" s="14"/>
+      <c r="B91" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="18" t="s">
+      <c r="C91" s="15"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="16"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2562,7 +2595,7 @@
       <c r="D93" s="1"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="G93" s="19" t="s">
+      <c r="G93" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2575,7 +2608,7 @@
       <c r="D94" s="1"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
-      <c r="G94" s="19" t="s">
+      <c r="G94" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2588,7 +2621,7 @@
       <c r="D95" s="1"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
-      <c r="G95" s="19" t="s">
+      <c r="G95" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2601,7 +2634,7 @@
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
-      <c r="G96" s="19" t="s">
+      <c r="G96" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2614,7 +2647,7 @@
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="19" t="s">
+      <c r="G97" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2627,20 +2660,20 @@
       <c r="D98" s="2"/>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
-      <c r="G98" s="19" t="s">
+      <c r="G98" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="15"/>
+      <c r="A99" s="14"/>
       <c r="B99" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="18" t="s">
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2668,7 +2701,7 @@
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="G101" s="19" t="s">
+      <c r="G101" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2681,7 +2714,7 @@
       <c r="D102" s="1"/>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="G102" s="19" t="s">
+      <c r="G102" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2694,7 +2727,7 @@
       <c r="D103" s="1"/>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
-      <c r="G103" s="19" t="s">
+      <c r="G103" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2707,7 +2740,7 @@
       <c r="D104" s="1"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
-      <c r="G104" s="19" t="s">
+      <c r="G104" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2720,7 +2753,7 @@
       <c r="D105" s="1"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="G105" s="19" t="s">
+      <c r="G105" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2733,20 +2766,20 @@
       <c r="D106" s="1"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="G106" s="19" t="s">
+      <c r="G106" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="15"/>
+      <c r="A107" s="14"/>
       <c r="B107" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C107" s="16"/>
-      <c r="D107" s="16"/>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
-      <c r="G107" s="18" t="s">
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="16"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2774,7 +2807,7 @@
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
-      <c r="G109" s="19" t="s">
+      <c r="G109" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2787,7 +2820,7 @@
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="19" t="s">
+      <c r="G110" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2800,7 +2833,7 @@
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
-      <c r="G111" s="19" t="s">
+      <c r="G111" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2813,7 +2846,7 @@
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
-      <c r="G112" s="19" t="s">
+      <c r="G112" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2826,7 +2859,7 @@
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
-      <c r="G113" s="19" t="s">
+      <c r="G113" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2839,20 +2872,20 @@
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
-      <c r="G114" s="19" t="s">
+      <c r="G114" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="15"/>
+      <c r="A115" s="14"/>
       <c r="B115" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C115" s="16"/>
-      <c r="D115" s="16"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="G115" s="18" t="s">
+      <c r="C115" s="15"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="17" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2880,7 +2913,7 @@
       <c r="D117" s="1"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
-      <c r="G117" s="19" t="s">
+      <c r="G117" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2893,7 +2926,7 @@
       <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
-      <c r="G118" s="19" t="s">
+      <c r="G118" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2906,7 +2939,7 @@
       <c r="D119" s="1"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
-      <c r="G119" s="19" t="s">
+      <c r="G119" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2919,7 +2952,7 @@
       <c r="D120" s="1"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
-      <c r="G120" s="19" t="s">
+      <c r="G120" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2932,7 +2965,7 @@
       <c r="D121" s="1"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
-      <c r="G121" s="19" t="s">
+      <c r="G121" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2945,20 +2978,20 @@
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
-      <c r="G122" s="19" t="s">
+      <c r="G122" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="15"/>
+      <c r="A123" s="14"/>
       <c r="B123" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C123" s="16"/>
-      <c r="D123" s="16"/>
-      <c r="E123" s="17"/>
-      <c r="F123" s="17"/>
-      <c r="G123" s="18" t="s">
+      <c r="C123" s="15"/>
+      <c r="D123" s="15"/>
+      <c r="E123" s="16"/>
+      <c r="F123" s="16"/>
+      <c r="G123" s="17" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.06e - Minor changes in sensor_scheduler and changes to analysis tool include stop button, baud rate selection, Save As... moved to menu-strip
</commit_message>
<xml_diff>
--- a/Source Code/MemoryMap.xlsx
+++ b/Source Code/MemoryMap.xlsx
@@ -164,9 +164,6 @@
     <t>Pin for RW line</t>
   </si>
   <si>
-    <t>ENABLE</t>
-  </si>
-  <si>
     <t>Pin for enable line</t>
   </si>
   <si>
@@ -630,6 +627,9 @@
   </si>
   <si>
     <t>SS1</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -893,12 +893,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,15 +1196,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1231,108 +1231,108 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1352,10 +1352,10 @@
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1373,9 +1373,9 @@
         <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G13" s="20"/>
+        <v>174</v>
+      </c>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -1392,9 +1392,9 @@
         <v>9</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G14" s="21"/>
+        <v>174</v>
+      </c>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
@@ -1411,9 +1411,9 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G15" s="20"/>
+        <v>174</v>
+      </c>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
@@ -1432,995 +1432,995 @@
       <c r="F16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>200</v>
+      <c r="G16" s="19" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>197</v>
+        <v>183</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E19" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>184</v>
-      </c>
       <c r="G19" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="F30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="18" t="s">
         <v>177</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="F31" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G31" s="18" t="s">
         <v>177</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="F36" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="F37" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="16"/>
       <c r="F51" s="16"/>
       <c r="G51" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="14"/>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
       <c r="E59" s="16"/>
       <c r="F59" s="16"/>
       <c r="G59" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="14"/>
       <c r="B67" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
       <c r="E67" s="16"/>
       <c r="F67" s="16"/>
       <c r="G67" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="14"/>
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15"/>
       <c r="E75" s="16"/>
       <c r="F75" s="16"/>
       <c r="G75" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D76" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E76" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="F76" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="F76" s="8" t="s">
-        <v>187</v>
-      </c>
       <c r="G76" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D77" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E77" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="F77" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G77" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="F78" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G78" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E79" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E79" s="4" t="s">
-        <v>193</v>
-      </c>
       <c r="F79" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G79" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G80" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G81" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
       <c r="G82" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
       <c r="B83" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="16"/>
       <c r="F83" s="16"/>
       <c r="G83" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2548,10 +2548,10 @@
         <v>17</v>
       </c>
       <c r="D90" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>37</v>
@@ -2561,438 +2561,438 @@
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="14"/>
       <c r="B91" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
       <c r="E91" s="16"/>
       <c r="F91" s="16"/>
       <c r="G91" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
       <c r="G92" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
       <c r="G97" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="14"/>
       <c r="B99" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C99" s="15"/>
       <c r="D99" s="15"/>
       <c r="E99" s="16"/>
       <c r="F99" s="16"/>
       <c r="G99" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
       <c r="G100" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
       <c r="G101" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
       <c r="G103" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
       <c r="G104" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="10"/>
       <c r="B105" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
       <c r="G105" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
       <c r="G106" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="14"/>
       <c r="B107" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="15"/>
       <c r="E107" s="16"/>
       <c r="F107" s="16"/>
       <c r="G107" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
       <c r="G108" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
       <c r="B109" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
       <c r="G109" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="10"/>
       <c r="B110" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
       <c r="G112" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="10"/>
       <c r="B113" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="14"/>
       <c r="B115" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C115" s="15"/>
       <c r="D115" s="15"/>
       <c r="E115" s="16"/>
       <c r="F115" s="16"/>
       <c r="G115" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
       <c r="G116" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
       <c r="G117" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="10"/>
       <c r="B119" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="10"/>
       <c r="B122" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
       <c r="G122" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="14"/>
       <c r="B123" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C123" s="15"/>
       <c r="D123" s="15"/>
       <c r="E123" s="16"/>
       <c r="F123" s="16"/>
       <c r="G123" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.07 - Minor upgrades to Testing Terminal and testing changes to main system
</commit_message>
<xml_diff>
--- a/Source Code/MemoryMap.xlsx
+++ b/Source Code/MemoryMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="210">
   <si>
     <t>SS</t>
   </si>
@@ -557,9 +557,6 @@
     <t>USART1</t>
   </si>
   <si>
-    <t>Not in use atm</t>
-  </si>
-  <si>
     <t>LED_GREEN</t>
   </si>
   <si>
@@ -630,23 +627,43 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>GSM_E</t>
+  </si>
+  <si>
+    <t>GPS_E</t>
+  </si>
+  <si>
+    <t>MODULE_E</t>
+  </si>
+  <si>
+    <t>GSM enable (active low)</t>
+  </si>
+  <si>
+    <t>GPS enable (active low)</t>
+  </si>
+  <si>
+    <t>Module enable (on wait off)</t>
+  </si>
+  <si>
+    <t>GSM/GPRS/GPS</t>
+  </si>
+  <si>
+    <t>Used by GSM/GPRS/GPS</t>
+  </si>
+  <si>
+    <t>Used for RS232 out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -672,7 +689,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,12 +698,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -808,15 +837,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -873,32 +893,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,186 +1216,186 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="27" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="19" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="18" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="19" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="18" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="18" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>200</v>
+      <c r="G12" s="7" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="1" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1372,14 +1407,14 @@
       <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1391,14 +1426,14 @@
       <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1413,11 +1448,11 @@
       <c r="F15" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1426,216 +1461,216 @@
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="19" t="s">
-        <v>199</v>
+      <c r="G16" s="14" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="20" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="19" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E19" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G18" s="18" t="s">
+      <c r="F19" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="18" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="19" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="18" t="s">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="19" t="s">
         <v>74</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="18" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="1" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="19" t="s">
         <v>75</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="18" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="1" t="s">
+      <c r="A25" s="23"/>
+      <c r="B25" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="18" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="23"/>
+      <c r="B26" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="18" t="s">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="1" t="s">
+      <c r="A27" s="24"/>
+      <c r="B27" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17" t="s">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="1" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="18" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="1" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1650,13 +1685,13 @@
       <c r="F30" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G30" s="18" t="s">
-        <v>177</v>
+      <c r="G30" s="13" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="19" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1671,67 +1706,67 @@
       <c r="F31" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G31" s="18" t="s">
-        <v>177</v>
+      <c r="G31" s="13" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="1" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="19" t="s">
         <v>66</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="18" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="1" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="18" t="s">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="23"/>
+      <c r="B34" s="19" t="s">
         <v>68</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="18" t="s">
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="17" t="s">
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1740,17 +1775,19 @@
       <c r="D36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G36" s="9"/>
+      <c r="G36" s="7" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="1" t="s">
+      <c r="A37" s="23"/>
+      <c r="B37" s="19" t="s">
         <v>94</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1759,694 +1796,714 @@
       <c r="D37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G37" s="18"/>
+      <c r="G37" s="13" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="1" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="19" t="s">
         <v>95</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="18" t="s">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="1" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="23"/>
+      <c r="B40" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="C40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="1" t="s">
+      <c r="A41" s="23"/>
+      <c r="B41" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="C41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="B42" s="1" t="s">
+      <c r="A42" s="23"/>
+      <c r="B42" s="19" t="s">
         <v>99</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="18" t="s">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
-      <c r="B43" s="1" t="s">
+      <c r="A43" s="24"/>
+      <c r="B43" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="17" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="1" t="s">
+      <c r="A45" s="23"/>
+      <c r="B45" s="19" t="s">
         <v>102</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="18" t="s">
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="1" t="s">
+      <c r="A46" s="23"/>
+      <c r="B46" s="19" t="s">
         <v>103</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="18" t="s">
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="1" t="s">
+      <c r="A47" s="23"/>
+      <c r="B47" s="19" t="s">
         <v>104</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="18" t="s">
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="1" t="s">
+      <c r="A48" s="23"/>
+      <c r="B48" s="19" t="s">
         <v>105</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="18" t="s">
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="1" t="s">
+      <c r="A49" s="23"/>
+      <c r="B49" s="19" t="s">
         <v>106</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="18" t="s">
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="B50" s="1" t="s">
+      <c r="A50" s="23"/>
+      <c r="B50" s="19" t="s">
         <v>107</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="18" t="s">
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15" t="s">
+      <c r="A51" s="24"/>
+      <c r="B51" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="17" t="s">
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9" t="s">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="B53" s="1" t="s">
+      <c r="A53" s="23"/>
+      <c r="B53" s="19" t="s">
         <v>110</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="18" t="s">
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="1" t="s">
+      <c r="A54" s="23"/>
+      <c r="B54" s="19" t="s">
         <v>111</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="18" t="s">
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="B55" s="1" t="s">
+      <c r="A55" s="23"/>
+      <c r="B55" s="19" t="s">
         <v>112</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="18" t="s">
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="B56" s="1" t="s">
+      <c r="A56" s="23"/>
+      <c r="B56" s="19" t="s">
         <v>113</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="18" t="s">
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="1" t="s">
+      <c r="A57" s="23"/>
+      <c r="B57" s="19" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="18" t="s">
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="B58" s="1" t="s">
+      <c r="A58" s="23"/>
+      <c r="B58" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="18" t="s">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="14"/>
-      <c r="B59" s="1" t="s">
+      <c r="A59" s="24"/>
+      <c r="B59" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="17" t="s">
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="9" t="s">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="1" t="s">
+      <c r="A61" s="23"/>
+      <c r="B61" s="19" t="s">
         <v>118</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="18" t="s">
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="1" t="s">
+      <c r="A62" s="23"/>
+      <c r="B62" s="19" t="s">
         <v>119</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="18" t="s">
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-      <c r="B63" s="1" t="s">
+      <c r="A63" s="23"/>
+      <c r="B63" s="19" t="s">
         <v>120</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="18" t="s">
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="B64" s="1" t="s">
+      <c r="A64" s="23"/>
+      <c r="B64" s="19" t="s">
         <v>121</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="18" t="s">
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
-      <c r="B65" s="1" t="s">
+      <c r="A65" s="23"/>
+      <c r="B65" s="19" t="s">
         <v>122</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="18" t="s">
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
-      <c r="B66" s="1" t="s">
+      <c r="A66" s="23"/>
+      <c r="B66" s="19" t="s">
         <v>123</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="18" t="s">
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="1" t="s">
+      <c r="A67" s="24"/>
+      <c r="B67" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="17" t="s">
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="9" t="s">
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
-      <c r="B69" s="1" t="s">
+      <c r="A69" s="23"/>
+      <c r="B69" s="19" t="s">
         <v>126</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="18" t="s">
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="10"/>
-      <c r="B70" s="1" t="s">
+      <c r="A70" s="23"/>
+      <c r="B70" s="19" t="s">
         <v>127</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="18" t="s">
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="10"/>
-      <c r="B71" s="1" t="s">
+      <c r="A71" s="23"/>
+      <c r="B71" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="18" t="s">
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
-      <c r="B72" s="1" t="s">
+      <c r="A72" s="23"/>
+      <c r="B72" s="19" t="s">
         <v>129</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="18" t="s">
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
-      <c r="B73" s="1" t="s">
+      <c r="A73" s="23"/>
+      <c r="B73" s="19" t="s">
         <v>130</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="18" t="s">
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="B74" s="1" t="s">
+      <c r="A74" s="23"/>
+      <c r="B74" s="19" t="s">
         <v>131</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="18" t="s">
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
-      <c r="B75" s="1" t="s">
+      <c r="A75" s="24"/>
+      <c r="B75" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="17" t="s">
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="F76" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F76" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="G76" s="9" t="s">
+      <c r="G76" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-      <c r="B77" s="1" t="s">
+      <c r="A77" s="23"/>
+      <c r="B77" s="19" t="s">
         <v>134</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D77" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G77" s="18" t="s">
+      <c r="F77" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G77" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
-      <c r="B78" s="1" t="s">
+      <c r="A78" s="23"/>
+      <c r="B78" s="19" t="s">
         <v>135</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D78" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G78" s="18" t="s">
+      <c r="F78" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G78" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
-      <c r="B79" s="1" t="s">
+      <c r="A79" s="23"/>
+      <c r="B79" s="19" t="s">
         <v>136</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D79" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E79" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G79" s="18" t="s">
+      <c r="F79" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G79" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="10"/>
-      <c r="B80" s="1" t="s">
+      <c r="A80" s="23"/>
+      <c r="B80" s="19" t="s">
         <v>137</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G80" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G80" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
-      <c r="B81" s="1" t="s">
+      <c r="A81" s="23"/>
+      <c r="B81" s="19" t="s">
         <v>138</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="G81" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G81" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
-      <c r="B82" s="1" t="s">
+      <c r="A82" s="23"/>
+      <c r="B82" s="19" t="s">
         <v>139</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="18" t="s">
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="14"/>
-      <c r="B83" s="1" t="s">
+      <c r="A83" s="24"/>
+      <c r="B83" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="17" t="s">
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E84" s="8" t="s">
+      <c r="E84" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="F84" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G84" s="9"/>
+      <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="B85" s="1" t="s">
+      <c r="A85" s="23"/>
+      <c r="B85" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -2455,17 +2512,17 @@
       <c r="D85" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F85" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G85" s="18"/>
+      <c r="G85" s="13"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="10"/>
-      <c r="B86" s="1" t="s">
+      <c r="A86" s="23"/>
+      <c r="B86" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -2474,17 +2531,17 @@
       <c r="D86" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F86" s="4" t="s">
+      <c r="F86" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G86" s="18"/>
+      <c r="G86" s="13"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="10"/>
-      <c r="B87" s="1" t="s">
+      <c r="A87" s="23"/>
+      <c r="B87" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2493,17 +2550,17 @@
       <c r="D87" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F87" s="4" t="s">
+      <c r="F87" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G87" s="18"/>
+      <c r="G87" s="13"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="10"/>
-      <c r="B88" s="1" t="s">
+      <c r="A88" s="23"/>
+      <c r="B88" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -2512,17 +2569,17 @@
       <c r="D88" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="F88" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G88" s="11"/>
+      <c r="G88" s="8"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="10"/>
-      <c r="B89" s="1" t="s">
+      <c r="A89" s="23"/>
+      <c r="B89" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -2531,473 +2588,488 @@
       <c r="D89" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E89" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="F89" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G89" s="11"/>
+      <c r="G89" s="8"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="10"/>
-      <c r="B90" s="2" t="s">
+      <c r="A90" s="23"/>
+      <c r="B90" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E90" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="F90" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G90" s="12"/>
+      <c r="G90" s="9"/>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="14"/>
-      <c r="B91" s="15" t="s">
+      <c r="A91" s="24"/>
+      <c r="B91" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="16"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="17" t="s">
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B92" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="7"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="9" t="s">
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
-      <c r="B93" s="1" t="s">
+      <c r="A93" s="23"/>
+      <c r="B93" s="19" t="s">
         <v>142</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="18" t="s">
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="10"/>
-      <c r="B94" s="1" t="s">
+      <c r="A94" s="23"/>
+      <c r="B94" s="19" t="s">
         <v>143</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="18" t="s">
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
-      <c r="B95" s="1" t="s">
+      <c r="A95" s="23"/>
+      <c r="B95" s="19" t="s">
         <v>144</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="18" t="s">
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="10"/>
-      <c r="B96" s="1" t="s">
+      <c r="A96" s="23"/>
+      <c r="B96" s="19" t="s">
         <v>145</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
-      <c r="G96" s="18" t="s">
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="10"/>
-      <c r="B97" s="1" t="s">
+      <c r="A97" s="23"/>
+      <c r="B97" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="18" t="s">
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
-      <c r="B98" s="1" t="s">
+      <c r="A98" s="23"/>
+      <c r="B98" s="19" t="s">
         <v>147</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="18" t="s">
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="14"/>
-      <c r="B99" s="1" t="s">
+      <c r="A99" s="24"/>
+      <c r="B99" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="C99" s="15"/>
-      <c r="D99" s="15"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="17" t="s">
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+      <c r="A100" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B100" s="7" t="s">
+      <c r="B100" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="9" t="s">
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="10"/>
-      <c r="B101" s="1" t="s">
+      <c r="A101" s="23"/>
+      <c r="B101" s="19" t="s">
         <v>150</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="18" t="s">
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="10"/>
-      <c r="B102" s="1" t="s">
+      <c r="A102" s="23"/>
+      <c r="B102" s="19" t="s">
         <v>151</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="4"/>
-      <c r="G102" s="18" t="s">
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="10"/>
-      <c r="B103" s="1" t="s">
+      <c r="A103" s="23"/>
+      <c r="B103" s="19" t="s">
         <v>152</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="18" t="s">
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="10"/>
-      <c r="B104" s="1" t="s">
+      <c r="A104" s="23"/>
+      <c r="B104" s="19" t="s">
         <v>153</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="18" t="s">
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
-      <c r="B105" s="1" t="s">
+      <c r="A105" s="23"/>
+      <c r="B105" s="19" t="s">
         <v>154</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="18" t="s">
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
-      <c r="B106" s="1" t="s">
+      <c r="A106" s="23"/>
+      <c r="B106" s="19" t="s">
         <v>155</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4"/>
-      <c r="G106" s="18" t="s">
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="14"/>
-      <c r="B107" s="1" t="s">
+      <c r="A107" s="24"/>
+      <c r="B107" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="16"/>
-      <c r="F107" s="16"/>
-      <c r="G107" s="17" t="s">
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B108" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="9" t="s">
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
-      <c r="B109" s="1" t="s">
+      <c r="A109" s="23"/>
+      <c r="B109" s="19" t="s">
         <v>158</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="G109" s="18" t="s">
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="10"/>
-      <c r="B110" s="1" t="s">
+      <c r="A110" s="23"/>
+      <c r="B110" s="19" t="s">
         <v>159</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="18" t="s">
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="10"/>
-      <c r="B111" s="1" t="s">
+      <c r="A111" s="23"/>
+      <c r="B111" s="19" t="s">
         <v>160</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
-      <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="18" t="s">
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="10"/>
-      <c r="B112" s="1" t="s">
+      <c r="A112" s="23"/>
+      <c r="B112" s="19" t="s">
         <v>161</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="18" t="s">
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="10"/>
-      <c r="B113" s="1" t="s">
+      <c r="A113" s="23"/>
+      <c r="B113" s="19" t="s">
         <v>162</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4"/>
-      <c r="G113" s="18" t="s">
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="10"/>
-      <c r="B114" s="1" t="s">
+      <c r="A114" s="23"/>
+      <c r="B114" s="19" t="s">
         <v>163</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4"/>
-      <c r="G114" s="18" t="s">
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="14"/>
-      <c r="B115" s="1" t="s">
+      <c r="A115" s="24"/>
+      <c r="B115" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="16"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="17" t="s">
+      <c r="C115" s="10"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
+      <c r="G115" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
+      <c r="A116" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B116" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="9" t="s">
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="10"/>
-      <c r="B117" s="1" t="s">
+      <c r="A117" s="23"/>
+      <c r="B117" s="19" t="s">
         <v>166</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
-      <c r="G117" s="18" t="s">
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="10"/>
-      <c r="B118" s="1" t="s">
+      <c r="A118" s="23"/>
+      <c r="B118" s="19" t="s">
         <v>167</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
-      <c r="E118" s="4"/>
-      <c r="F118" s="4"/>
-      <c r="G118" s="18" t="s">
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="10"/>
-      <c r="B119" s="1" t="s">
+      <c r="A119" s="23"/>
+      <c r="B119" s="19" t="s">
         <v>168</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="18" t="s">
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="10"/>
-      <c r="B120" s="1" t="s">
+      <c r="A120" s="23"/>
+      <c r="B120" s="19" t="s">
         <v>169</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="18" t="s">
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="10"/>
-      <c r="B121" s="1" t="s">
+      <c r="A121" s="23"/>
+      <c r="B121" s="19" t="s">
         <v>170</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="18" t="s">
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="10"/>
-      <c r="B122" s="1" t="s">
+      <c r="A122" s="23"/>
+      <c r="B122" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="18" t="s">
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="14"/>
-      <c r="B123" s="1" t="s">
+      <c r="A123" s="24"/>
+      <c r="B123" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="C123" s="15"/>
-      <c r="D123" s="15"/>
-      <c r="E123" s="16"/>
-      <c r="F123" s="16"/>
-      <c r="G123" s="17" t="s">
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
+      <c r="G123" s="12" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="16">
+    <mergeCell ref="A116:A123"/>
+    <mergeCell ref="A76:A83"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="A92:A99"/>
+    <mergeCell ref="A100:A107"/>
+    <mergeCell ref="A108:A115"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="A68:A75"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A28:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.098 Added car_driver using PORTJ
</commit_message>
<xml_diff>
--- a/Source Code/MemoryMap.xlsx
+++ b/Source Code/MemoryMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Skole Opgaver\ICT Engineering\7th Semester\Bachelor Project\Source Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\Atmel Studio\6.2\VROOM (Git)\Source Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="220">
   <si>
     <t>SS</t>
   </si>
@@ -654,6 +654,36 @@
   </si>
   <si>
     <t>Used for RS232 out</t>
+  </si>
+  <si>
+    <t>Cancel button</t>
+  </si>
+  <si>
+    <t>Alarm button</t>
+  </si>
+  <si>
+    <t>car_panel</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
+  </si>
+  <si>
+    <t>ALARM</t>
+  </si>
+  <si>
+    <t>CONTROL</t>
+  </si>
+  <si>
+    <t>STATUS_RED</t>
+  </si>
+  <si>
+    <t>STATUS_BLUE</t>
+  </si>
+  <si>
+    <t>STATUS_GREEN</t>
+  </si>
+  <si>
+    <t>Blue LED</t>
   </si>
 </sst>
 </file>
@@ -918,6 +948,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -930,10 +964,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,56 +1246,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="18" t="s">
@@ -1275,12 +1305,10 @@
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
@@ -1288,12 +1316,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="19" t="s">
         <v>53</v>
       </c>
@@ -1301,12 +1327,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="19" t="s">
         <v>54</v>
       </c>
@@ -1314,12 +1338,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="19" t="s">
         <v>55</v>
       </c>
@@ -1327,12 +1349,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="19" t="s">
         <v>56</v>
       </c>
@@ -1340,12 +1360,10 @@
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="19" t="s">
         <v>57</v>
       </c>
@@ -1353,12 +1371,10 @@
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="19" t="s">
         <v>58</v>
       </c>
@@ -1366,12 +1382,10 @@
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -1394,7 +1408,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="19" t="s">
         <v>2</v>
       </c>
@@ -1413,7 +1427,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="20" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1446,7 @@
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="19" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1465,7 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
@@ -1472,7 +1486,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="20" t="s">
         <v>59</v>
       </c>
@@ -1493,7 +1507,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="19" t="s">
         <v>60</v>
       </c>
@@ -1514,7 +1528,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>61</v>
       </c>
@@ -1535,7 +1549,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="24" t="s">
         <v>70</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -1550,7 +1564,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="19" t="s">
         <v>72</v>
       </c>
@@ -1563,7 +1577,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="19" t="s">
         <v>73</v>
       </c>
@@ -1576,7 +1590,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="19" t="s">
         <v>74</v>
       </c>
@@ -1589,7 +1603,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="19" t="s">
         <v>75</v>
       </c>
@@ -1602,7 +1616,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="19" t="s">
         <v>76</v>
       </c>
@@ -1615,7 +1629,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="19" t="s">
         <v>77</v>
       </c>
@@ -1628,7 +1642,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="19" t="s">
         <v>78</v>
       </c>
@@ -1641,7 +1655,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -1656,7 +1670,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="19" t="s">
         <v>63</v>
       </c>
@@ -1669,7 +1683,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="19" t="s">
         <v>64</v>
       </c>
@@ -1690,7 +1704,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="19" t="s">
         <v>65</v>
       </c>
@@ -1711,7 +1725,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="19" t="s">
         <v>66</v>
       </c>
@@ -1724,7 +1738,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="19" t="s">
         <v>67</v>
       </c>
@@ -1737,7 +1751,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="19" t="s">
         <v>68</v>
       </c>
@@ -1750,7 +1764,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="21" t="s">
         <v>69</v>
       </c>
@@ -1763,7 +1777,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="18" t="s">
@@ -1786,7 +1800,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="19" t="s">
         <v>94</v>
       </c>
@@ -1807,7 +1821,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="19" t="s">
         <v>95</v>
       </c>
@@ -1820,7 +1834,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="19" t="s">
         <v>96</v>
       </c>
@@ -1839,7 +1853,7 @@
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="19" t="s">
         <v>97</v>
       </c>
@@ -1858,7 +1872,7 @@
       <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="19" t="s">
         <v>98</v>
       </c>
@@ -1877,7 +1891,7 @@
       <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="19" t="s">
         <v>99</v>
       </c>
@@ -1890,7 +1904,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="19" t="s">
         <v>100</v>
       </c>
@@ -1903,7 +1917,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="24" t="s">
         <v>80</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -1918,7 +1932,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="19" t="s">
         <v>102</v>
       </c>
@@ -1931,7 +1945,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="19" t="s">
         <v>103</v>
       </c>
@@ -1944,7 +1958,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="19" t="s">
         <v>104</v>
       </c>
@@ -1957,7 +1971,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="19" t="s">
         <v>105</v>
       </c>
@@ -1970,7 +1984,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="19" t="s">
         <v>106</v>
       </c>
@@ -1983,7 +1997,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="19" t="s">
         <v>107</v>
       </c>
@@ -1996,7 +2010,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="24"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="21" t="s">
         <v>108</v>
       </c>
@@ -2009,7 +2023,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="24" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="18" t="s">
@@ -2024,7 +2038,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="19" t="s">
         <v>110</v>
       </c>
@@ -2037,7 +2051,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="19" t="s">
         <v>111</v>
       </c>
@@ -2050,7 +2064,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="19" t="s">
         <v>112</v>
       </c>
@@ -2063,7 +2077,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
+      <c r="A56" s="25"/>
       <c r="B56" s="19" t="s">
         <v>113</v>
       </c>
@@ -2076,7 +2090,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="19" t="s">
         <v>114</v>
       </c>
@@ -2089,7 +2103,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="19" t="s">
         <v>115</v>
       </c>
@@ -2102,7 +2116,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="19" t="s">
         <v>116</v>
       </c>
@@ -2115,7 +2129,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="24" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="18" t="s">
@@ -2130,7 +2144,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="19" t="s">
         <v>118</v>
       </c>
@@ -2143,7 +2157,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="19" t="s">
         <v>119</v>
       </c>
@@ -2156,7 +2170,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="19" t="s">
         <v>120</v>
       </c>
@@ -2169,7 +2183,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="19" t="s">
         <v>121</v>
       </c>
@@ -2182,7 +2196,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
+      <c r="A65" s="25"/>
       <c r="B65" s="19" t="s">
         <v>122</v>
       </c>
@@ -2195,7 +2209,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="19" t="s">
         <v>123</v>
       </c>
@@ -2208,7 +2222,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="24"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="19" t="s">
         <v>124</v>
       </c>
@@ -2221,35 +2235,47 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="22" t="s">
+      <c r="A68" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="C68" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
+      <c r="A69" s="25"/>
       <c r="B69" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="19" t="s">
         <v>127</v>
       </c>
@@ -2262,20 +2288,26 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G71" s="13"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="19" t="s">
         <v>129</v>
       </c>
@@ -2288,46 +2320,64 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
+      <c r="A73" s="25"/>
       <c r="B73" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G73" s="13"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C74" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G74" s="13"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="24"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="C75" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="G75" s="12"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="22" t="s">
+      <c r="A76" s="24" t="s">
         <v>84</v>
       </c>
       <c r="B76" s="18" t="s">
@@ -2350,7 +2400,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="25"/>
       <c r="B77" s="19" t="s">
         <v>134</v>
       </c>
@@ -2371,7 +2421,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
+      <c r="A78" s="25"/>
       <c r="B78" s="19" t="s">
         <v>135</v>
       </c>
@@ -2392,7 +2442,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
+      <c r="A79" s="25"/>
       <c r="B79" s="19" t="s">
         <v>136</v>
       </c>
@@ -2413,7 +2463,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="19" t="s">
         <v>137</v>
       </c>
@@ -2434,7 +2484,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
+      <c r="A81" s="25"/>
       <c r="B81" s="19" t="s">
         <v>138</v>
       </c>
@@ -2455,7 +2505,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="19" t="s">
         <v>139</v>
       </c>
@@ -2468,7 +2518,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="24"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="19" t="s">
         <v>140</v>
       </c>
@@ -2481,7 +2531,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
+      <c r="A84" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B84" s="18" t="s">
@@ -2502,7 +2552,7 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="23"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="19" t="s">
         <v>13</v>
       </c>
@@ -2521,7 +2571,7 @@
       <c r="G85" s="13"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="23"/>
+      <c r="A86" s="25"/>
       <c r="B86" s="19" t="s">
         <v>12</v>
       </c>
@@ -2540,7 +2590,7 @@
       <c r="G86" s="13"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="23"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="19" t="s">
         <v>11</v>
       </c>
@@ -2559,7 +2609,7 @@
       <c r="G87" s="13"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="23"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="19" t="s">
         <v>30</v>
       </c>
@@ -2578,7 +2628,7 @@
       <c r="G88" s="8"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="23"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="19" t="s">
         <v>31</v>
       </c>
@@ -2597,7 +2647,7 @@
       <c r="G89" s="8"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="20" t="s">
         <v>32</v>
       </c>
@@ -2616,7 +2666,7 @@
       <c r="G90" s="9"/>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="24"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="21" t="s">
         <v>48</v>
       </c>
@@ -2629,7 +2679,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="22" t="s">
+      <c r="A92" s="24" t="s">
         <v>85</v>
       </c>
       <c r="B92" s="18" t="s">
@@ -2644,7 +2694,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="19" t="s">
         <v>142</v>
       </c>
@@ -2657,7 +2707,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="19" t="s">
         <v>143</v>
       </c>
@@ -2670,7 +2720,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="19" t="s">
         <v>144</v>
       </c>
@@ -2683,7 +2733,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
+      <c r="A96" s="25"/>
       <c r="B96" s="19" t="s">
         <v>145</v>
       </c>
@@ -2696,7 +2746,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="23"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="19" t="s">
         <v>146</v>
       </c>
@@ -2709,7 +2759,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="23"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="19" t="s">
         <v>147</v>
       </c>
@@ -2722,7 +2772,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="24"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="19" t="s">
         <v>148</v>
       </c>
@@ -2735,7 +2785,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
+      <c r="A100" s="24" t="s">
         <v>86</v>
       </c>
       <c r="B100" s="18" t="s">
@@ -2750,7 +2800,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="23"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="19" t="s">
         <v>150</v>
       </c>
@@ -2763,7 +2813,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="23"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="19" t="s">
         <v>151</v>
       </c>
@@ -2776,7 +2826,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="23"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="19" t="s">
         <v>152</v>
       </c>
@@ -2789,7 +2839,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="23"/>
+      <c r="A104" s="25"/>
       <c r="B104" s="19" t="s">
         <v>153</v>
       </c>
@@ -2802,7 +2852,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="23"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="19" t="s">
         <v>154</v>
       </c>
@@ -2815,7 +2865,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="23"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="19" t="s">
         <v>155</v>
       </c>
@@ -2828,7 +2878,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="24"/>
+      <c r="A107" s="26"/>
       <c r="B107" s="19" t="s">
         <v>156</v>
       </c>
@@ -2841,7 +2891,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="22" t="s">
+      <c r="A108" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B108" s="18" t="s">
@@ -2856,7 +2906,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="23"/>
+      <c r="A109" s="25"/>
       <c r="B109" s="19" t="s">
         <v>158</v>
       </c>
@@ -2869,7 +2919,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="23"/>
+      <c r="A110" s="25"/>
       <c r="B110" s="19" t="s">
         <v>159</v>
       </c>
@@ -2882,7 +2932,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="23"/>
+      <c r="A111" s="25"/>
       <c r="B111" s="19" t="s">
         <v>160</v>
       </c>
@@ -2895,7 +2945,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="23"/>
+      <c r="A112" s="25"/>
       <c r="B112" s="19" t="s">
         <v>161</v>
       </c>
@@ -2908,7 +2958,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="23"/>
+      <c r="A113" s="25"/>
       <c r="B113" s="19" t="s">
         <v>162</v>
       </c>
@@ -2921,7 +2971,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="23"/>
+      <c r="A114" s="25"/>
       <c r="B114" s="19" t="s">
         <v>163</v>
       </c>
@@ -2934,7 +2984,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="24"/>
+      <c r="A115" s="26"/>
       <c r="B115" s="19" t="s">
         <v>164</v>
       </c>
@@ -2947,7 +2997,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="22" t="s">
+      <c r="A116" s="24" t="s">
         <v>88</v>
       </c>
       <c r="B116" s="18" t="s">
@@ -2962,7 +3012,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="23"/>
+      <c r="A117" s="25"/>
       <c r="B117" s="19" t="s">
         <v>166</v>
       </c>
@@ -2975,7 +3025,7 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="23"/>
+      <c r="A118" s="25"/>
       <c r="B118" s="19" t="s">
         <v>167</v>
       </c>
@@ -2988,7 +3038,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="23"/>
+      <c r="A119" s="25"/>
       <c r="B119" s="19" t="s">
         <v>168</v>
       </c>
@@ -3001,7 +3051,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="23"/>
+      <c r="A120" s="25"/>
       <c r="B120" s="19" t="s">
         <v>169</v>
       </c>
@@ -3014,7 +3064,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
+      <c r="A121" s="25"/>
       <c r="B121" s="19" t="s">
         <v>170</v>
       </c>
@@ -3027,7 +3077,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="23"/>
+      <c r="A122" s="25"/>
       <c r="B122" s="19" t="s">
         <v>171</v>
       </c>
@@ -3040,7 +3090,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="24"/>
+      <c r="A123" s="26"/>
       <c r="B123" s="21" t="s">
         <v>172</v>
       </c>
@@ -3054,22 +3104,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="A68:A75"/>
     <mergeCell ref="A116:A123"/>
     <mergeCell ref="A76:A83"/>
     <mergeCell ref="A84:A91"/>
     <mergeCell ref="A92:A99"/>
     <mergeCell ref="A100:A107"/>
     <mergeCell ref="A108:A115"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A59"/>
-    <mergeCell ref="A60:A67"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A28:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v0.200 - Changed sensor_scheduler to scheduler for the whole system. Eliminated comm problem.
</commit_message>
<xml_diff>
--- a/Source Code/MemoryMap.xlsx
+++ b/Source Code/MemoryMap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\Atmel Studio\6.2\VROOM (Git)\Source Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Skole Opgaver\ICT Engineering\7th Semester\Bachelor Project\Source Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="228">
   <si>
     <t>SS</t>
   </si>
@@ -557,12 +557,6 @@
     <t>USART1</t>
   </si>
   <si>
-    <t>LED_GREEN</t>
-  </si>
-  <si>
-    <t>LED_RED</t>
-  </si>
-  <si>
     <t>Green LED</t>
   </si>
   <si>
@@ -575,33 +569,6 @@
     <t>lop</t>
   </si>
   <si>
-    <t>BTN_PIN0</t>
-  </si>
-  <si>
-    <t>Button 0</t>
-  </si>
-  <si>
-    <t>btn_led_lcd</t>
-  </si>
-  <si>
-    <t>BTN_PIN1</t>
-  </si>
-  <si>
-    <t>Button 1</t>
-  </si>
-  <si>
-    <t>BTN_PIN2</t>
-  </si>
-  <si>
-    <t>Button 2</t>
-  </si>
-  <si>
-    <t>BTN_PIN3</t>
-  </si>
-  <si>
-    <t>Button 3</t>
-  </si>
-  <si>
     <t>LOP_GREEN</t>
   </si>
   <si>
@@ -611,15 +578,6 @@
     <t>LOP_YELLOW</t>
   </si>
   <si>
-    <t>Possible SS3</t>
-  </si>
-  <si>
-    <t>Possible SS4</t>
-  </si>
-  <si>
-    <t>Possible SS5</t>
-  </si>
-  <si>
     <t>SS2</t>
   </si>
   <si>
@@ -684,6 +642,72 @@
   </si>
   <si>
     <t>Blue LED</t>
+  </si>
+  <si>
+    <t>R2R_BIT0</t>
+  </si>
+  <si>
+    <t>R2R_LED0</t>
+  </si>
+  <si>
+    <t>R2R_BIT1</t>
+  </si>
+  <si>
+    <t>R2R_BIT2</t>
+  </si>
+  <si>
+    <t>R2R_BIT3</t>
+  </si>
+  <si>
+    <t>R2R_LED1</t>
+  </si>
+  <si>
+    <t>R2R_LED2</t>
+  </si>
+  <si>
+    <t>R2R_LED3</t>
+  </si>
+  <si>
+    <t>Bit 0 for R2R DAC</t>
+  </si>
+  <si>
+    <t>Bit 1 for R2R DAC</t>
+  </si>
+  <si>
+    <t>Bit 2 for R2R DAC</t>
+  </si>
+  <si>
+    <t>Bit 3 for R2R DAC</t>
+  </si>
+  <si>
+    <t>LED 0 (from right)</t>
+  </si>
+  <si>
+    <t>LED 1 (from right)</t>
+  </si>
+  <si>
+    <t>LED 2 (from right)</t>
+  </si>
+  <si>
+    <t>LED 3 (from right)</t>
+  </si>
+  <si>
+    <t>r2r_led</t>
+  </si>
+  <si>
+    <t>For DEBUG</t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>Possible SS3 Not used</t>
+  </si>
+  <si>
+    <t>Possible SS4 Not used</t>
+  </si>
+  <si>
+    <t>Possible SS5 Not used</t>
   </si>
 </sst>
 </file>
@@ -952,6 +976,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -960,9 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1246,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:A75"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,15 +1285,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
@@ -1295,7 +1319,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="18" t="s">
@@ -1308,7 +1332,7 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
@@ -1319,7 +1343,7 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="19" t="s">
         <v>53</v>
       </c>
@@ -1330,7 +1354,7 @@
       <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="19" t="s">
         <v>54</v>
       </c>
@@ -1341,7 +1365,7 @@
       <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="19" t="s">
         <v>55</v>
       </c>
@@ -1352,7 +1376,7 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="19" t="s">
         <v>56</v>
       </c>
@@ -1363,7 +1387,7 @@
       <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="19" t="s">
         <v>57</v>
       </c>
@@ -1374,7 +1398,7 @@
       <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="19" t="s">
         <v>58</v>
       </c>
@@ -1385,7 +1409,7 @@
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -1404,11 +1428,11 @@
         <v>173</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="19" t="s">
         <v>2</v>
       </c>
@@ -1427,7 +1451,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="20" t="s">
         <v>4</v>
       </c>
@@ -1446,7 +1470,7 @@
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="19" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1489,7 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
@@ -1482,11 +1506,11 @@
         <v>28</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="20" t="s">
         <v>59</v>
       </c>
@@ -1494,20 +1518,20 @@
         <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="19" t="s">
         <v>60</v>
       </c>
@@ -1515,20 +1539,20 @@
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>182</v>
-      </c>
       <c r="G18" s="13" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="19" t="s">
         <v>61</v>
       </c>
@@ -1536,20 +1560,20 @@
         <v>17</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -1564,7 +1588,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="19" t="s">
         <v>72</v>
       </c>
@@ -1577,7 +1601,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="19" t="s">
         <v>73</v>
       </c>
@@ -1590,7 +1614,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="19" t="s">
         <v>74</v>
       </c>
@@ -1603,7 +1627,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="19" t="s">
         <v>75</v>
       </c>
@@ -1616,7 +1640,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="19" t="s">
         <v>76</v>
       </c>
@@ -1629,7 +1653,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="19" t="s">
         <v>77</v>
       </c>
@@ -1642,7 +1666,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="19" t="s">
         <v>78</v>
       </c>
@@ -1655,7 +1679,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -1670,7 +1694,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="19" t="s">
         <v>63</v>
       </c>
@@ -1683,7 +1707,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="19" t="s">
         <v>64</v>
       </c>
@@ -1700,11 +1724,11 @@
         <v>176</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="19" t="s">
         <v>65</v>
       </c>
@@ -1721,11 +1745,11 @@
         <v>176</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="19" t="s">
         <v>66</v>
       </c>
@@ -1738,7 +1762,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="19" t="s">
         <v>67</v>
       </c>
@@ -1751,7 +1775,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="19" t="s">
         <v>68</v>
       </c>
@@ -1764,7 +1788,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="21" t="s">
         <v>69</v>
       </c>
@@ -1777,7 +1801,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="25" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="18" t="s">
@@ -1796,11 +1820,11 @@
         <v>175</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="19" t="s">
         <v>94</v>
       </c>
@@ -1817,11 +1841,11 @@
         <v>175</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="19" t="s">
         <v>95</v>
       </c>
@@ -1834,7 +1858,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="19" t="s">
         <v>96</v>
       </c>
@@ -1842,18 +1866,18 @@
         <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="19" t="s">
         <v>97</v>
       </c>
@@ -1861,18 +1885,18 @@
         <v>17</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="19" t="s">
         <v>98</v>
       </c>
@@ -1880,18 +1904,18 @@
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="19" t="s">
         <v>99</v>
       </c>
@@ -1900,11 +1924,11 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="13" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="19" t="s">
         <v>100</v>
       </c>
@@ -1912,12 +1936,12 @@
       <c r="D43" s="10"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="12" t="s">
-        <v>49</v>
+      <c r="G43" s="13" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="25" t="s">
         <v>80</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -1932,7 +1956,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="19" t="s">
         <v>102</v>
       </c>
@@ -1945,7 +1969,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="19" t="s">
         <v>103</v>
       </c>
@@ -1958,7 +1982,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="19" t="s">
         <v>104</v>
       </c>
@@ -1971,7 +1995,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="19" t="s">
         <v>105</v>
       </c>
@@ -1984,7 +2008,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="19" t="s">
         <v>106</v>
       </c>
@@ -1997,7 +2021,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="19" t="s">
         <v>107</v>
       </c>
@@ -2010,7 +2034,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="21" t="s">
         <v>108</v>
       </c>
@@ -2023,7 +2047,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="25" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="18" t="s">
@@ -2038,7 +2062,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="19" t="s">
         <v>110</v>
       </c>
@@ -2051,7 +2075,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="19" t="s">
         <v>111</v>
       </c>
@@ -2064,7 +2088,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="19" t="s">
         <v>112</v>
       </c>
@@ -2077,7 +2101,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="19" t="s">
         <v>113</v>
       </c>
@@ -2090,7 +2114,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="19" t="s">
         <v>114</v>
       </c>
@@ -2103,7 +2127,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="19" t="s">
         <v>115</v>
       </c>
@@ -2116,7 +2140,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="19" t="s">
         <v>116</v>
       </c>
@@ -2129,113 +2153,177 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="25" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
+      <c r="C60" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>222</v>
+      </c>
       <c r="G60" s="7" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+      <c r="C61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G61" s="13" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
+      <c r="A62" s="26"/>
       <c r="B62" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
+      <c r="C62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G62" s="13" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="C63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G63" s="13" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
+      <c r="C64" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G64" s="13" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="25"/>
+      <c r="A65" s="26"/>
       <c r="B65" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="C65" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G65" s="13" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
+      <c r="A66" s="26"/>
       <c r="B66" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
+      <c r="C66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G66" s="13" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="26"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
+      <c r="C67" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="G67" s="12" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="25" t="s">
         <v>83</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -2245,18 +2333,18 @@
         <v>18</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
+      <c r="A69" s="26"/>
       <c r="B69" s="19" t="s">
         <v>126</v>
       </c>
@@ -2264,18 +2352,18 @@
         <v>18</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
+      <c r="A70" s="26"/>
       <c r="B70" s="19" t="s">
         <v>127</v>
       </c>
@@ -2284,11 +2372,11 @@
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="13" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="19" t="s">
         <v>128</v>
       </c>
@@ -2296,18 +2384,18 @@
         <v>17</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G71" s="13"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="19" t="s">
         <v>129</v>
       </c>
@@ -2316,11 +2404,11 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="13" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="25"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="19" t="s">
         <v>130</v>
       </c>
@@ -2328,18 +2416,18 @@
         <v>17</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G73" s="13"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
+      <c r="A74" s="26"/>
       <c r="B74" s="19" t="s">
         <v>131</v>
       </c>
@@ -2347,18 +2435,18 @@
         <v>17</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G74" s="13"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="26"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="19" t="s">
         <v>132</v>
       </c>
@@ -2366,146 +2454,86 @@
         <v>17</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G75" s="12"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="24" t="s">
+      <c r="A76" s="25" t="s">
         <v>84</v>
       </c>
       <c r="B76" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="7"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="25"/>
+      <c r="A77" s="26"/>
       <c r="B77" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G77" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="13"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="25"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="13"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G79" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="13"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
+      <c r="A80" s="26"/>
       <c r="B80" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="13"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
+      <c r="A81" s="26"/>
       <c r="B81" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G81" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="13"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
+      <c r="A82" s="26"/>
       <c r="B82" s="19" t="s">
         <v>139</v>
       </c>
@@ -2513,12 +2541,10 @@
       <c r="D82" s="2"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="G82" s="13"/>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="26"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="19" t="s">
         <v>140</v>
       </c>
@@ -2526,12 +2552,10 @@
       <c r="D83" s="10"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
-      <c r="G83" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="G83" s="12"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="24" t="s">
+      <c r="A84" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B84" s="18" t="s">
@@ -2549,10 +2573,12 @@
       <c r="F84" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G84" s="7"/>
+      <c r="G84" s="7" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="19" t="s">
         <v>13</v>
       </c>
@@ -2568,10 +2594,12 @@
       <c r="F85" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G85" s="13"/>
+      <c r="G85" s="13" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="25"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="19" t="s">
         <v>12</v>
       </c>
@@ -2587,10 +2615,12 @@
       <c r="F86" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G86" s="13"/>
+      <c r="G86" s="13" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="19" t="s">
         <v>11</v>
       </c>
@@ -2606,10 +2636,12 @@
       <c r="F87" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G87" s="13"/>
+      <c r="G87" s="13" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
+      <c r="A88" s="26"/>
       <c r="B88" s="19" t="s">
         <v>30</v>
       </c>
@@ -2625,10 +2657,12 @@
       <c r="F88" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G88" s="8"/>
+      <c r="G88" s="8" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
+      <c r="A89" s="26"/>
       <c r="B89" s="19" t="s">
         <v>31</v>
       </c>
@@ -2644,10 +2678,12 @@
       <c r="F89" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G89" s="8"/>
+      <c r="G89" s="8" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
+      <c r="A90" s="26"/>
       <c r="B90" s="20" t="s">
         <v>32</v>
       </c>
@@ -2655,7 +2691,7 @@
         <v>17</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>46</v>
@@ -2663,10 +2699,12 @@
       <c r="F90" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G90" s="9"/>
+      <c r="G90" s="9" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="26"/>
+      <c r="A91" s="27"/>
       <c r="B91" s="21" t="s">
         <v>48</v>
       </c>
@@ -2674,12 +2712,12 @@
       <c r="D91" s="10"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
-      <c r="G91" s="12" t="s">
-        <v>49</v>
+      <c r="G91" s="13" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="24" t="s">
+      <c r="A92" s="25" t="s">
         <v>85</v>
       </c>
       <c r="B92" s="18" t="s">
@@ -2694,7 +2732,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
+      <c r="A93" s="26"/>
       <c r="B93" s="19" t="s">
         <v>142</v>
       </c>
@@ -2707,7 +2745,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="19" t="s">
         <v>143</v>
       </c>
@@ -2720,7 +2758,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
+      <c r="A95" s="26"/>
       <c r="B95" s="19" t="s">
         <v>144</v>
       </c>
@@ -2733,7 +2771,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="25"/>
+      <c r="A96" s="26"/>
       <c r="B96" s="19" t="s">
         <v>145</v>
       </c>
@@ -2746,7 +2784,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
+      <c r="A97" s="26"/>
       <c r="B97" s="19" t="s">
         <v>146</v>
       </c>
@@ -2759,7 +2797,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="25"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="19" t="s">
         <v>147</v>
       </c>
@@ -2772,7 +2810,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="26"/>
+      <c r="A99" s="27"/>
       <c r="B99" s="19" t="s">
         <v>148</v>
       </c>
@@ -2785,7 +2823,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="24" t="s">
+      <c r="A100" s="25" t="s">
         <v>86</v>
       </c>
       <c r="B100" s="18" t="s">
@@ -2800,7 +2838,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="25"/>
+      <c r="A101" s="26"/>
       <c r="B101" s="19" t="s">
         <v>150</v>
       </c>
@@ -2813,7 +2851,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="25"/>
+      <c r="A102" s="26"/>
       <c r="B102" s="19" t="s">
         <v>151</v>
       </c>
@@ -2826,7 +2864,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="25"/>
+      <c r="A103" s="26"/>
       <c r="B103" s="19" t="s">
         <v>152</v>
       </c>
@@ -2839,7 +2877,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="25"/>
+      <c r="A104" s="26"/>
       <c r="B104" s="19" t="s">
         <v>153</v>
       </c>
@@ -2852,7 +2890,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="25"/>
+      <c r="A105" s="26"/>
       <c r="B105" s="19" t="s">
         <v>154</v>
       </c>
@@ -2865,7 +2903,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="25"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="19" t="s">
         <v>155</v>
       </c>
@@ -2878,7 +2916,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="26"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="19" t="s">
         <v>156</v>
       </c>
@@ -2891,7 +2929,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="24" t="s">
+      <c r="A108" s="25" t="s">
         <v>87</v>
       </c>
       <c r="B108" s="18" t="s">
@@ -2906,7 +2944,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="25"/>
+      <c r="A109" s="26"/>
       <c r="B109" s="19" t="s">
         <v>158</v>
       </c>
@@ -2919,7 +2957,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="25"/>
+      <c r="A110" s="26"/>
       <c r="B110" s="19" t="s">
         <v>159</v>
       </c>
@@ -2932,7 +2970,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="25"/>
+      <c r="A111" s="26"/>
       <c r="B111" s="19" t="s">
         <v>160</v>
       </c>
@@ -2945,7 +2983,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
+      <c r="A112" s="26"/>
       <c r="B112" s="19" t="s">
         <v>161</v>
       </c>
@@ -2958,7 +2996,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="25"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="19" t="s">
         <v>162</v>
       </c>
@@ -2971,7 +3009,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="25"/>
+      <c r="A114" s="26"/>
       <c r="B114" s="19" t="s">
         <v>163</v>
       </c>
@@ -2984,7 +3022,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="26"/>
+      <c r="A115" s="27"/>
       <c r="B115" s="19" t="s">
         <v>164</v>
       </c>
@@ -2997,7 +3035,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="24" t="s">
+      <c r="A116" s="25" t="s">
         <v>88</v>
       </c>
       <c r="B116" s="18" t="s">
@@ -3012,7 +3050,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="25"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="19" t="s">
         <v>166</v>
       </c>
@@ -3025,7 +3063,7 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="25"/>
+      <c r="A118" s="26"/>
       <c r="B118" s="19" t="s">
         <v>167</v>
       </c>
@@ -3038,7 +3076,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
+      <c r="A119" s="26"/>
       <c r="B119" s="19" t="s">
         <v>168</v>
       </c>
@@ -3051,7 +3089,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
+      <c r="A120" s="26"/>
       <c r="B120" s="19" t="s">
         <v>169</v>
       </c>
@@ -3064,7 +3102,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="25"/>
+      <c r="A121" s="26"/>
       <c r="B121" s="19" t="s">
         <v>170</v>
       </c>
@@ -3077,7 +3115,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
+      <c r="A122" s="26"/>
       <c r="B122" s="19" t="s">
         <v>171</v>
       </c>
@@ -3090,7 +3128,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="26"/>
+      <c r="A123" s="27"/>
       <c r="B123" s="21" t="s">
         <v>172</v>
       </c>
@@ -3104,22 +3142,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A59"/>
-    <mergeCell ref="A60:A67"/>
-    <mergeCell ref="A68:A75"/>
     <mergeCell ref="A116:A123"/>
     <mergeCell ref="A76:A83"/>
     <mergeCell ref="A84:A91"/>
     <mergeCell ref="A92:A99"/>
     <mergeCell ref="A100:A107"/>
     <mergeCell ref="A108:A115"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A28:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added timeout counters in sim908 FPT setup so that it can run without simcard
</commit_message>
<xml_diff>
--- a/Source Code/MemoryMap.xlsx
+++ b/Source Code/MemoryMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="228">
   <si>
     <t>SS</t>
   </si>
@@ -976,9 +976,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -987,6 +984,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,15 +1285,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="18" t="s">
@@ -1329,10 +1329,12 @@
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="G4" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="19" t="s">
         <v>52</v>
       </c>
@@ -1340,10 +1342,12 @@
       <c r="D5" s="1"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="19" t="s">
         <v>53</v>
       </c>
@@ -1351,10 +1355,12 @@
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="19" t="s">
         <v>54</v>
       </c>
@@ -1362,10 +1368,12 @@
       <c r="D7" s="1"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="19" t="s">
         <v>55</v>
       </c>
@@ -1373,10 +1381,12 @@
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="19" t="s">
         <v>56</v>
       </c>
@@ -1384,10 +1394,12 @@
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="19" t="s">
         <v>57</v>
       </c>
@@ -1395,10 +1407,12 @@
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="19" t="s">
         <v>58</v>
       </c>
@@ -1406,10 +1420,12 @@
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="18" t="s">
@@ -1432,7 +1448,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="19" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1467,7 @@
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="20" t="s">
         <v>4</v>
       </c>
@@ -1470,7 +1486,7 @@
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="19" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1505,7 @@
       <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
@@ -1510,7 +1526,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="20" t="s">
         <v>59</v>
       </c>
@@ -1531,7 +1547,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="19" t="s">
         <v>60</v>
       </c>
@@ -1552,7 +1568,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="19" t="s">
         <v>61</v>
       </c>
@@ -1573,7 +1589,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="24" t="s">
         <v>70</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -1588,7 +1604,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="19" t="s">
         <v>72</v>
       </c>
@@ -1601,7 +1617,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="19" t="s">
         <v>73</v>
       </c>
@@ -1614,7 +1630,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="19" t="s">
         <v>74</v>
       </c>
@@ -1627,7 +1643,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="19" t="s">
         <v>75</v>
       </c>
@@ -1640,7 +1656,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="19" t="s">
         <v>76</v>
       </c>
@@ -1653,7 +1669,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="19" t="s">
         <v>77</v>
       </c>
@@ -1666,7 +1682,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="19" t="s">
         <v>78</v>
       </c>
@@ -1679,7 +1695,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -1694,7 +1710,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="19" t="s">
         <v>63</v>
       </c>
@@ -1707,7 +1723,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="19" t="s">
         <v>64</v>
       </c>
@@ -1728,7 +1744,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="19" t="s">
         <v>65</v>
       </c>
@@ -1749,7 +1765,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="19" t="s">
         <v>66</v>
       </c>
@@ -1762,7 +1778,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="19" t="s">
         <v>67</v>
       </c>
@@ -1775,7 +1791,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="19" t="s">
         <v>68</v>
       </c>
@@ -1788,7 +1804,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="21" t="s">
         <v>69</v>
       </c>
@@ -1801,7 +1817,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="18" t="s">
@@ -1824,7 +1840,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="19" t="s">
         <v>94</v>
       </c>
@@ -1845,7 +1861,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="19" t="s">
         <v>95</v>
       </c>
@@ -1858,7 +1874,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="19" t="s">
         <v>96</v>
       </c>
@@ -1877,7 +1893,7 @@
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="19" t="s">
         <v>97</v>
       </c>
@@ -1896,7 +1912,7 @@
       <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="19" t="s">
         <v>98</v>
       </c>
@@ -1915,7 +1931,7 @@
       <c r="G41" s="13"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="19" t="s">
         <v>99</v>
       </c>
@@ -1928,7 +1944,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="19" t="s">
         <v>100</v>
       </c>
@@ -1941,7 +1957,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="24" t="s">
         <v>80</v>
       </c>
       <c r="B44" s="18" t="s">
@@ -1956,7 +1972,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="19" t="s">
         <v>102</v>
       </c>
@@ -1969,7 +1985,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="19" t="s">
         <v>103</v>
       </c>
@@ -1982,7 +1998,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="19" t="s">
         <v>104</v>
       </c>
@@ -1995,7 +2011,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="19" t="s">
         <v>105</v>
       </c>
@@ -2008,7 +2024,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="19" t="s">
         <v>106</v>
       </c>
@@ -2021,7 +2037,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="19" t="s">
         <v>107</v>
       </c>
@@ -2034,7 +2050,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="27"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="21" t="s">
         <v>108</v>
       </c>
@@ -2047,7 +2063,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="24" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="18" t="s">
@@ -2062,7 +2078,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="19" t="s">
         <v>110</v>
       </c>
@@ -2075,7 +2091,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="19" t="s">
         <v>111</v>
       </c>
@@ -2088,7 +2104,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="19" t="s">
         <v>112</v>
       </c>
@@ -2101,7 +2117,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="25"/>
       <c r="B56" s="19" t="s">
         <v>113</v>
       </c>
@@ -2114,7 +2130,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="19" t="s">
         <v>114</v>
       </c>
@@ -2127,7 +2143,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="19" t="s">
         <v>115</v>
       </c>
@@ -2140,7 +2156,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="27"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="19" t="s">
         <v>116</v>
       </c>
@@ -2153,7 +2169,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="24" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="18" t="s">
@@ -2176,7 +2192,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="19" t="s">
         <v>118</v>
       </c>
@@ -2197,7 +2213,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="19" t="s">
         <v>119</v>
       </c>
@@ -2218,7 +2234,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="19" t="s">
         <v>120</v>
       </c>
@@ -2239,7 +2255,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="19" t="s">
         <v>121</v>
       </c>
@@ -2260,7 +2276,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
+      <c r="A65" s="25"/>
       <c r="B65" s="19" t="s">
         <v>122</v>
       </c>
@@ -2281,7 +2297,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="26"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="19" t="s">
         <v>123</v>
       </c>
@@ -2302,7 +2318,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="27"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="19" t="s">
         <v>124</v>
       </c>
@@ -2323,7 +2339,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -2344,7 +2360,7 @@
       <c r="G68" s="7"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="26"/>
+      <c r="A69" s="25"/>
       <c r="B69" s="19" t="s">
         <v>126</v>
       </c>
@@ -2363,7 +2379,7 @@
       <c r="G69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="19" t="s">
         <v>127</v>
       </c>
@@ -2376,7 +2392,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="19" t="s">
         <v>128</v>
       </c>
@@ -2395,7 +2411,7 @@
       <c r="G71" s="13"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="19" t="s">
         <v>129</v>
       </c>
@@ -2408,7 +2424,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="26"/>
+      <c r="A73" s="25"/>
       <c r="B73" s="19" t="s">
         <v>130</v>
       </c>
@@ -2427,7 +2443,7 @@
       <c r="G73" s="13"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="19" t="s">
         <v>131</v>
       </c>
@@ -2446,7 +2462,7 @@
       <c r="G74" s="13"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="27"/>
+      <c r="A75" s="26"/>
       <c r="B75" s="19" t="s">
         <v>132</v>
       </c>
@@ -2465,7 +2481,7 @@
       <c r="G75" s="12"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="25" t="s">
+      <c r="A76" s="24" t="s">
         <v>84</v>
       </c>
       <c r="B76" s="18" t="s">
@@ -2475,10 +2491,12 @@
       <c r="D76" s="5"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
-      <c r="G76" s="7"/>
+      <c r="G76" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
+      <c r="A77" s="25"/>
       <c r="B77" s="19" t="s">
         <v>134</v>
       </c>
@@ -2486,10 +2504,12 @@
       <c r="D77" s="1"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="13"/>
+      <c r="G77" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
+      <c r="A78" s="25"/>
       <c r="B78" s="19" t="s">
         <v>135</v>
       </c>
@@ -2497,10 +2517,12 @@
       <c r="D78" s="1"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="13"/>
+      <c r="G78" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="26"/>
+      <c r="A79" s="25"/>
       <c r="B79" s="19" t="s">
         <v>136</v>
       </c>
@@ -2508,10 +2530,12 @@
       <c r="D79" s="1"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
-      <c r="G79" s="13"/>
+      <c r="G79" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="19" t="s">
         <v>137</v>
       </c>
@@ -2519,10 +2543,12 @@
       <c r="D80" s="1"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="13"/>
+      <c r="G80" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
+      <c r="A81" s="25"/>
       <c r="B81" s="19" t="s">
         <v>138</v>
       </c>
@@ -2530,10 +2556,12 @@
       <c r="D81" s="1"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
-      <c r="G81" s="13"/>
+      <c r="G81" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="19" t="s">
         <v>139</v>
       </c>
@@ -2541,10 +2569,12 @@
       <c r="D82" s="2"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="13"/>
+      <c r="G82" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="27"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="19" t="s">
         <v>140</v>
       </c>
@@ -2552,10 +2582,12 @@
       <c r="D83" s="10"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
-      <c r="G83" s="12"/>
+      <c r="G83" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="25" t="s">
+      <c r="A84" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B84" s="18" t="s">
@@ -2578,7 +2610,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="19" t="s">
         <v>13</v>
       </c>
@@ -2599,7 +2631,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="26"/>
+      <c r="A86" s="25"/>
       <c r="B86" s="19" t="s">
         <v>12</v>
       </c>
@@ -2620,7 +2652,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="19" t="s">
         <v>11</v>
       </c>
@@ -2641,7 +2673,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="19" t="s">
         <v>30</v>
       </c>
@@ -2662,7 +2694,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
+      <c r="A89" s="25"/>
       <c r="B89" s="19" t="s">
         <v>31</v>
       </c>
@@ -2683,7 +2715,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="26"/>
+      <c r="A90" s="25"/>
       <c r="B90" s="20" t="s">
         <v>32</v>
       </c>
@@ -2704,7 +2736,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="27"/>
+      <c r="A91" s="26"/>
       <c r="B91" s="21" t="s">
         <v>48</v>
       </c>
@@ -2717,7 +2749,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="25" t="s">
+      <c r="A92" s="24" t="s">
         <v>85</v>
       </c>
       <c r="B92" s="18" t="s">
@@ -2732,7 +2764,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="26"/>
+      <c r="A93" s="25"/>
       <c r="B93" s="19" t="s">
         <v>142</v>
       </c>
@@ -2745,7 +2777,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
+      <c r="A94" s="25"/>
       <c r="B94" s="19" t="s">
         <v>143</v>
       </c>
@@ -2758,7 +2790,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
+      <c r="A95" s="25"/>
       <c r="B95" s="19" t="s">
         <v>144</v>
       </c>
@@ -2771,7 +2803,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
+      <c r="A96" s="25"/>
       <c r="B96" s="19" t="s">
         <v>145</v>
       </c>
@@ -2784,7 +2816,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
+      <c r="A97" s="25"/>
       <c r="B97" s="19" t="s">
         <v>146</v>
       </c>
@@ -2797,7 +2829,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
+      <c r="A98" s="25"/>
       <c r="B98" s="19" t="s">
         <v>147</v>
       </c>
@@ -2810,7 +2842,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="27"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="19" t="s">
         <v>148</v>
       </c>
@@ -2823,7 +2855,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="24" t="s">
         <v>86</v>
       </c>
       <c r="B100" s="18" t="s">
@@ -2838,7 +2870,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
+      <c r="A101" s="25"/>
       <c r="B101" s="19" t="s">
         <v>150</v>
       </c>
@@ -2851,7 +2883,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
+      <c r="A102" s="25"/>
       <c r="B102" s="19" t="s">
         <v>151</v>
       </c>
@@ -2864,7 +2896,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="26"/>
+      <c r="A103" s="25"/>
       <c r="B103" s="19" t="s">
         <v>152</v>
       </c>
@@ -2877,7 +2909,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="26"/>
+      <c r="A104" s="25"/>
       <c r="B104" s="19" t="s">
         <v>153</v>
       </c>
@@ -2890,7 +2922,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
+      <c r="A105" s="25"/>
       <c r="B105" s="19" t="s">
         <v>154</v>
       </c>
@@ -2903,7 +2935,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="26"/>
+      <c r="A106" s="25"/>
       <c r="B106" s="19" t="s">
         <v>155</v>
       </c>
@@ -2916,7 +2948,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="27"/>
+      <c r="A107" s="26"/>
       <c r="B107" s="19" t="s">
         <v>156</v>
       </c>
@@ -2929,7 +2961,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="25" t="s">
+      <c r="A108" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B108" s="18" t="s">
@@ -2944,7 +2976,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
+      <c r="A109" s="25"/>
       <c r="B109" s="19" t="s">
         <v>158</v>
       </c>
@@ -2957,7 +2989,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="26"/>
+      <c r="A110" s="25"/>
       <c r="B110" s="19" t="s">
         <v>159</v>
       </c>
@@ -2970,7 +3002,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
+      <c r="A111" s="25"/>
       <c r="B111" s="19" t="s">
         <v>160</v>
       </c>
@@ -2983,7 +3015,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
+      <c r="A112" s="25"/>
       <c r="B112" s="19" t="s">
         <v>161</v>
       </c>
@@ -2996,7 +3028,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="26"/>
+      <c r="A113" s="25"/>
       <c r="B113" s="19" t="s">
         <v>162</v>
       </c>
@@ -3009,7 +3041,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
+      <c r="A114" s="25"/>
       <c r="B114" s="19" t="s">
         <v>163</v>
       </c>
@@ -3022,7 +3054,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="27"/>
+      <c r="A115" s="26"/>
       <c r="B115" s="19" t="s">
         <v>164</v>
       </c>
@@ -3035,7 +3067,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="25" t="s">
+      <c r="A116" s="24" t="s">
         <v>88</v>
       </c>
       <c r="B116" s="18" t="s">
@@ -3050,7 +3082,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="26"/>
+      <c r="A117" s="25"/>
       <c r="B117" s="19" t="s">
         <v>166</v>
       </c>
@@ -3063,7 +3095,7 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="26"/>
+      <c r="A118" s="25"/>
       <c r="B118" s="19" t="s">
         <v>167</v>
       </c>
@@ -3076,7 +3108,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
+      <c r="A119" s="25"/>
       <c r="B119" s="19" t="s">
         <v>168</v>
       </c>
@@ -3089,7 +3121,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="26"/>
+      <c r="A120" s="25"/>
       <c r="B120" s="19" t="s">
         <v>169</v>
       </c>
@@ -3102,7 +3134,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="26"/>
+      <c r="A121" s="25"/>
       <c r="B121" s="19" t="s">
         <v>170</v>
       </c>
@@ -3115,7 +3147,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="26"/>
+      <c r="A122" s="25"/>
       <c r="B122" s="19" t="s">
         <v>171</v>
       </c>
@@ -3128,7 +3160,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="27"/>
+      <c r="A123" s="26"/>
       <c r="B123" s="21" t="s">
         <v>172</v>
       </c>
@@ -3142,22 +3174,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A59"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="A68:A75"/>
     <mergeCell ref="A116:A123"/>
     <mergeCell ref="A76:A83"/>
     <mergeCell ref="A84:A91"/>
     <mergeCell ref="A92:A99"/>
     <mergeCell ref="A100:A107"/>
     <mergeCell ref="A108:A115"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A44:A51"/>
-    <mergeCell ref="A52:A59"/>
-    <mergeCell ref="A60:A67"/>
-    <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A28:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>